<commit_message>
create entity in progress
</commit_message>
<xml_diff>
--- a/testData/CreateEntity/CreateEntity_DefaultValues_Test.xlsx
+++ b/testData/CreateEntity/CreateEntity_DefaultValues_Test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="133">
   <si>
     <t>WorflowName</t>
   </si>
@@ -395,6 +395,33 @@
   </si>
   <si>
     <t>CT: Wed, Apr 03, 2024 at 12:01 PM</t>
+  </si>
+  <si>
+    <t>CT: Fri, Apr 05, 2024 at 6:46 PM</t>
+  </si>
+  <si>
+    <t>CT: Fri, Apr 05, 2024 at 6:49 PM</t>
+  </si>
+  <si>
+    <t>CT: Fri, Apr 05, 2024 at 6:52 PM</t>
+  </si>
+  <si>
+    <t>CT: Sat, Apr 06, 2024 at 11:13 AM</t>
+  </si>
+  <si>
+    <t>CT: Sat, Apr 06, 2024 at 11:17 AM</t>
+  </si>
+  <si>
+    <t>CT: Sat, Apr 06, 2024 at 11:20 AM</t>
+  </si>
+  <si>
+    <t>CT: Sat, Apr 06, 2024 at 11:32 AM</t>
+  </si>
+  <si>
+    <t>CT: Sat, Apr 06, 2024 at 11:35 AM</t>
+  </si>
+  <si>
+    <t>CT: Sat, Apr 06, 2024 at 11:38 AM</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1144,7 @@
         <v>114</v>
       </c>
       <c r="BB2" t="s" s="2">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create Entity & Send Notification
</commit_message>
<xml_diff>
--- a/testData/CreateEntity/CreateEntity_DefaultValues_Test.xlsx
+++ b/testData/CreateEntity/CreateEntity_DefaultValues_Test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="149">
   <si>
     <t>WorflowName</t>
   </si>
@@ -461,6 +461,15 @@
   </si>
   <si>
     <t>CT: Fri, Jul 12, 2024 at 3:16 PM</t>
+  </si>
+  <si>
+    <t>CT: Mon, Jan 06, 2025 at 2:22 PM</t>
+  </si>
+  <si>
+    <t>CT: Mon, Jan 06, 2025 at 2:27 PM</t>
+  </si>
+  <si>
+    <t>CT: Mon, Jan 06, 2025 at 2:31 PM</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1192,7 @@
         <v>114</v>
       </c>
       <c r="BB2" t="s" s="2">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before demo on create entity&sendnotify
</commit_message>
<xml_diff>
--- a/testData/CreateEntity/CreateEntity_DefaultValues_Test.xlsx
+++ b/testData/CreateEntity/CreateEntity_DefaultValues_Test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="152">
   <si>
     <t>WorflowName</t>
   </si>
@@ -470,6 +470,15 @@
   </si>
   <si>
     <t>CT: Mon, Jan 06, 2025 at 2:31 PM</t>
+  </si>
+  <si>
+    <t>CT: Mon, Jan 06, 2025 at 6:55 PM</t>
+  </si>
+  <si>
+    <t>CT: Mon, Jan 06, 2025 at 7:00 PM</t>
+  </si>
+  <si>
+    <t>CT: Mon, Jan 06, 2025 at 7:04 PM</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1201,7 @@
         <v>114</v>
       </c>
       <c r="BB2" t="s" s="2">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>